<commit_message>
Added Pivot and First Tree Chart
</commit_message>
<xml_diff>
--- a/charts/ChartPlan.xlsx
+++ b/charts/ChartPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MattP\Desktop\Capstone\charts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mapeyton\OneDrive - American Medical Association\Desktop\Site\charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626DFDC6-4789-4527-827C-7D16F53BB9DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18240" yWindow="3165" windowWidth="24270" windowHeight="15435" firstSheet="3" activeTab="6" xr2:uid="{B37984B5-7E5B-4A29-BA31-35AC76D76266}"/>
+    <workbookView minimized="1" xWindow="11790" yWindow="0" windowWidth="17010" windowHeight="15600" firstSheet="3" activeTab="6" xr2:uid="{B37984B5-7E5B-4A29-BA31-35AC76D76266}"/>
   </bookViews>
   <sheets>
     <sheet name="Scratch" sheetId="1" r:id="rId1"/>
@@ -233,7 +233,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -459,6 +459,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -471,9 +474,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -15542,17 +15542,17 @@
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
-      <c r="D45" s="37" t="s">
+      <c r="D45" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="E45" s="37"/>
-      <c r="F45" s="37"/>
-      <c r="G45" s="38" t="s">
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="H45" s="38"/>
-      <c r="I45" s="38"/>
-      <c r="J45" s="38"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="8"/>
@@ -15967,26 +15967,26 @@
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B62" s="36" t="s">
+      <c r="B62" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C62" s="36"/>
-      <c r="D62" s="36"/>
-      <c r="E62" s="36" t="s">
+      <c r="C62" s="39"/>
+      <c r="D62" s="39"/>
+      <c r="E62" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="F62" s="36"/>
-      <c r="G62" s="36"/>
-      <c r="H62" s="36" t="s">
+      <c r="F62" s="39"/>
+      <c r="G62" s="39"/>
+      <c r="H62" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="I62" s="36"/>
-      <c r="J62" s="36"/>
-      <c r="K62" s="36" t="s">
+      <c r="I62" s="39"/>
+      <c r="J62" s="39"/>
+      <c r="K62" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="L62" s="36"/>
-      <c r="M62" s="36"/>
+      <c r="L62" s="39"/>
+      <c r="M62" s="39"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B63" s="1">
@@ -16568,21 +16568,21 @@
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B80" s="36" t="s">
+      <c r="B80" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="C80" s="36"/>
-      <c r="D80" s="36"/>
-      <c r="E80" s="36" t="s">
+      <c r="C80" s="39"/>
+      <c r="D80" s="39"/>
+      <c r="E80" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="F80" s="36"/>
-      <c r="G80" s="36"/>
-      <c r="H80" s="36" t="s">
+      <c r="F80" s="39"/>
+      <c r="G80" s="39"/>
+      <c r="H80" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="I80" s="36"/>
-      <c r="J80" s="36"/>
+      <c r="I80" s="39"/>
+      <c r="J80" s="39"/>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B81" s="1" t="s">
@@ -17318,17 +17318,17 @@
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
-      <c r="D29" s="37" t="s">
+      <c r="D29" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="38" t="s">
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="41"/>
     </row>
     <row r="30" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
@@ -17743,26 +17743,26 @@
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B46" s="36" t="s">
+      <c r="B46" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="36"/>
-      <c r="D46" s="36"/>
-      <c r="E46" s="36" t="s">
+      <c r="C46" s="39"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="F46" s="36"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="36" t="s">
+      <c r="F46" s="39"/>
+      <c r="G46" s="39"/>
+      <c r="H46" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
-      <c r="K46" s="36" t="s">
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
+      <c r="K46" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="L46" s="36"/>
-      <c r="M46" s="36"/>
+      <c r="L46" s="39"/>
+      <c r="M46" s="39"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B47" s="1">
@@ -18344,21 +18344,21 @@
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B64" s="36" t="s">
+      <c r="B64" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="C64" s="36"/>
-      <c r="D64" s="36"/>
-      <c r="E64" s="36" t="s">
+      <c r="C64" s="39"/>
+      <c r="D64" s="39"/>
+      <c r="E64" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="F64" s="36"/>
-      <c r="G64" s="36"/>
-      <c r="H64" s="36" t="s">
+      <c r="F64" s="39"/>
+      <c r="G64" s="39"/>
+      <c r="H64" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="I64" s="36"/>
-      <c r="J64" s="36"/>
+      <c r="I64" s="39"/>
+      <c r="J64" s="39"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
@@ -19240,21 +19240,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36" t="s">
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36" t="s">
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1">
@@ -20117,21 +20117,21 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="39" t="s">
+      <c r="B37" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="39"/>
-      <c r="D37" s="39"/>
-      <c r="E37" s="39" t="s">
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="F37" s="39"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="39" t="s">
+      <c r="F37" s="42"/>
+      <c r="G37" s="42"/>
+      <c r="H37" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="I37" s="39"/>
-      <c r="J37" s="39"/>
+      <c r="I37" s="42"/>
+      <c r="J37" s="42"/>
     </row>
     <row r="38" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -20583,21 +20583,21 @@
     </row>
     <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="39" t="s">
+      <c r="B54" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="C54" s="39"/>
-      <c r="D54" s="39"/>
-      <c r="E54" s="39" t="s">
+      <c r="C54" s="42"/>
+      <c r="D54" s="42"/>
+      <c r="E54" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="F54" s="39"/>
-      <c r="G54" s="39"/>
-      <c r="H54" s="39" t="s">
+      <c r="F54" s="42"/>
+      <c r="G54" s="42"/>
+      <c r="H54" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="I54" s="39"/>
-      <c r="J54" s="39"/>
+      <c r="I54" s="42"/>
+      <c r="J54" s="42"/>
     </row>
     <row r="55" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B55" s="1">
@@ -21067,7 +21067,7 @@
   <dimension ref="A3:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="G6" sqref="G6:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21078,26 +21078,26 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36" t="s">
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36" t="s">
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36" t="s">
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
@@ -21141,40 +21141,40 @@
       <c r="A5" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="40">
+      <c r="B5" s="36">
         <v>312779</v>
       </c>
-      <c r="C5" s="40">
+      <c r="C5" s="36">
         <v>293265</v>
       </c>
-      <c r="D5" s="40">
+      <c r="D5" s="36">
         <v>314744</v>
       </c>
-      <c r="E5" s="40">
+      <c r="E5" s="36">
         <v>1424</v>
       </c>
-      <c r="F5" s="40">
+      <c r="F5" s="36">
         <v>1641</v>
       </c>
-      <c r="G5" s="40">
+      <c r="G5" s="36">
         <v>1978.6</v>
       </c>
-      <c r="H5" s="40">
+      <c r="H5" s="36">
         <v>1307.7</v>
       </c>
-      <c r="I5" s="40">
+      <c r="I5" s="36">
         <v>1576.9</v>
       </c>
-      <c r="J5" s="40">
+      <c r="J5" s="36">
         <v>1838.9</v>
       </c>
-      <c r="K5" s="40">
+      <c r="K5" s="36">
         <v>2506.4</v>
       </c>
-      <c r="L5" s="40">
+      <c r="L5" s="36">
         <v>2904.1</v>
       </c>
-      <c r="M5" s="40">
+      <c r="M5" s="36">
         <v>3668.6</v>
       </c>
     </row>
@@ -21182,40 +21182,40 @@
       <c r="A6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="41">
+      <c r="B6" s="37">
         <v>34483</v>
       </c>
-      <c r="C6" s="41">
+      <c r="C6" s="37">
         <v>29409</v>
       </c>
-      <c r="D6" s="42">
+      <c r="D6" s="38">
         <v>31429</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="37">
         <v>31.7</v>
       </c>
-      <c r="F6" s="41">
+      <c r="F6" s="37">
         <v>31.5</v>
       </c>
-      <c r="G6" s="41">
+      <c r="G6" s="37">
         <v>40.6</v>
       </c>
-      <c r="H6" s="41">
+      <c r="H6" s="37">
         <v>27.7</v>
       </c>
-      <c r="I6" s="41">
+      <c r="I6" s="37">
         <v>29.9</v>
       </c>
-      <c r="J6" s="41">
+      <c r="J6" s="37">
         <v>35.700000000000003</v>
       </c>
-      <c r="K6" s="41">
+      <c r="K6" s="37">
         <v>98.3</v>
       </c>
-      <c r="L6" s="41">
+      <c r="L6" s="37">
         <v>105.3</v>
       </c>
-      <c r="M6" s="41">
+      <c r="M6" s="37">
         <v>127.9</v>
       </c>
     </row>
@@ -21223,40 +21223,40 @@
       <c r="A7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="41">
+      <c r="B7" s="37">
         <v>56030</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="37">
         <v>50387</v>
       </c>
-      <c r="D7" s="42">
+      <c r="D7" s="38">
         <v>54214</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="37">
         <v>251.7</v>
       </c>
-      <c r="F7" s="41">
+      <c r="F7" s="37">
         <v>268.39999999999998</v>
       </c>
-      <c r="G7" s="41">
+      <c r="G7" s="37">
         <v>354.3</v>
       </c>
-      <c r="H7" s="41">
+      <c r="H7" s="37">
         <v>210.5</v>
       </c>
-      <c r="I7" s="41">
+      <c r="I7" s="37">
         <v>261.5</v>
       </c>
-      <c r="J7" s="41">
+      <c r="J7" s="37">
         <v>315.5</v>
       </c>
-      <c r="K7" s="41">
+      <c r="K7" s="37">
         <v>783.1</v>
       </c>
-      <c r="L7" s="41">
+      <c r="L7" s="37">
         <v>846.1</v>
       </c>
-      <c r="M7" s="41">
+      <c r="M7" s="37">
         <v>1128.8</v>
       </c>
     </row>
@@ -21264,40 +21264,40 @@
       <c r="A8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="41">
+      <c r="B8" s="37">
         <v>1869</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="37">
         <v>2040</v>
       </c>
-      <c r="D8" s="42">
+      <c r="D8" s="38">
         <v>2153</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="37">
         <v>166.3</v>
       </c>
-      <c r="F8" s="41">
+      <c r="F8" s="37">
         <v>173.3</v>
       </c>
-      <c r="G8" s="41">
+      <c r="G8" s="37">
         <v>230.9</v>
       </c>
-      <c r="H8" s="41">
+      <c r="H8" s="37">
         <v>140.19999999999999</v>
       </c>
-      <c r="I8" s="41">
+      <c r="I8" s="37">
         <v>169.3</v>
       </c>
-      <c r="J8" s="41">
+      <c r="J8" s="37">
         <v>207.4</v>
       </c>
-      <c r="K8" s="41">
+      <c r="K8" s="37">
         <v>527.6</v>
       </c>
-      <c r="L8" s="41">
+      <c r="L8" s="37">
         <v>549.70000000000005</v>
       </c>
-      <c r="M8" s="41">
+      <c r="M8" s="37">
         <v>736.3</v>
       </c>
     </row>
@@ -21305,40 +21305,40 @@
       <c r="A9" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="41">
+      <c r="B9" s="37">
         <v>54161</v>
       </c>
-      <c r="C9" s="41">
+      <c r="C9" s="37">
         <v>48347</v>
       </c>
-      <c r="D9" s="42">
+      <c r="D9" s="38">
         <v>52061</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="37">
         <v>85.4</v>
       </c>
-      <c r="F9" s="41">
+      <c r="F9" s="37">
         <v>95.1</v>
       </c>
-      <c r="G9" s="41">
+      <c r="G9" s="37">
         <v>123.4</v>
       </c>
-      <c r="H9" s="41">
+      <c r="H9" s="37">
         <v>70.3</v>
       </c>
-      <c r="I9" s="41">
+      <c r="I9" s="37">
         <v>92.2</v>
       </c>
-      <c r="J9" s="41">
+      <c r="J9" s="37">
         <v>108.1</v>
       </c>
-      <c r="K9" s="41">
+      <c r="K9" s="37">
         <v>255.5</v>
       </c>
-      <c r="L9" s="41">
+      <c r="L9" s="37">
         <v>296.39999999999998</v>
       </c>
-      <c r="M9" s="41">
+      <c r="M9" s="37">
         <v>392.5</v>
       </c>
     </row>
@@ -21346,40 +21346,40 @@
       <c r="A10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="41">
+      <c r="B10" s="37">
         <v>12721</v>
       </c>
-      <c r="C10" s="41">
+      <c r="C10" s="37">
         <v>12715</v>
       </c>
-      <c r="D10" s="42">
+      <c r="D10" s="38">
         <v>14591</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="37">
         <v>13</v>
       </c>
-      <c r="F10" s="41">
+      <c r="F10" s="37">
         <v>14.7</v>
       </c>
-      <c r="G10" s="41">
+      <c r="G10" s="37">
         <v>19.7</v>
       </c>
-      <c r="H10" s="41">
+      <c r="H10" s="37">
         <v>11</v>
       </c>
-      <c r="I10" s="41">
+      <c r="I10" s="37">
         <v>13.7</v>
       </c>
-      <c r="J10" s="41">
+      <c r="J10" s="37">
         <v>16.5</v>
       </c>
-      <c r="K10" s="41">
+      <c r="K10" s="37">
         <v>32</v>
       </c>
-      <c r="L10" s="41">
+      <c r="L10" s="37">
         <v>37.700000000000003</v>
       </c>
-      <c r="M10" s="41">
+      <c r="M10" s="37">
         <v>47.8</v>
       </c>
     </row>
@@ -21387,40 +21387,40 @@
       <c r="A11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="41">
+      <c r="B11" s="37">
         <v>40774</v>
       </c>
-      <c r="C11" s="41">
+      <c r="C11" s="37">
         <v>38840</v>
       </c>
-      <c r="D11" s="42">
+      <c r="D11" s="38">
         <v>38861</v>
       </c>
-      <c r="E11" s="41">
+      <c r="E11" s="37">
         <v>817.2</v>
       </c>
-      <c r="F11" s="41">
+      <c r="F11" s="37">
         <v>986</v>
       </c>
-      <c r="G11" s="41">
+      <c r="G11" s="37">
         <v>1160.5</v>
       </c>
-      <c r="H11" s="41">
+      <c r="H11" s="37">
         <v>775.8</v>
       </c>
-      <c r="I11" s="41">
+      <c r="I11" s="37">
         <v>944.6</v>
       </c>
-      <c r="J11" s="41">
+      <c r="J11" s="37">
         <v>1102.3</v>
       </c>
-      <c r="K11" s="41">
+      <c r="K11" s="37">
         <v>1000.8</v>
       </c>
-      <c r="L11" s="41">
+      <c r="L11" s="37">
         <v>1238.9000000000001</v>
       </c>
-      <c r="M11" s="41">
+      <c r="M11" s="37">
         <v>1574.1</v>
       </c>
     </row>
@@ -21428,40 +21428,40 @@
       <c r="A12" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="41">
+      <c r="B12" s="37">
         <v>7150</v>
       </c>
-      <c r="C12" s="41">
+      <c r="C12" s="37">
         <v>7229</v>
       </c>
-      <c r="D12" s="42">
+      <c r="D12" s="38">
         <v>7113</v>
       </c>
-      <c r="E12" s="41">
+      <c r="E12" s="37">
         <v>689.3</v>
       </c>
-      <c r="F12" s="41">
+      <c r="F12" s="37">
         <v>838.3</v>
       </c>
-      <c r="G12" s="41">
+      <c r="G12" s="37">
         <v>977.1</v>
       </c>
-      <c r="H12" s="41">
+      <c r="H12" s="37">
         <v>658.4</v>
       </c>
-      <c r="I12" s="41">
+      <c r="I12" s="37">
         <v>802.8</v>
       </c>
-      <c r="J12" s="41">
+      <c r="J12" s="37">
         <v>926.7</v>
       </c>
-      <c r="K12" s="41">
+      <c r="K12" s="37">
         <v>790.1</v>
       </c>
-      <c r="L12" s="41">
+      <c r="L12" s="37">
         <v>1004.2</v>
       </c>
-      <c r="M12" s="41">
+      <c r="M12" s="37">
         <v>1281.5</v>
       </c>
     </row>
@@ -21469,40 +21469,40 @@
       <c r="A13" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="41">
+      <c r="B13" s="37">
         <v>33624</v>
       </c>
-      <c r="C13" s="41">
+      <c r="C13" s="37">
         <v>31611</v>
       </c>
-      <c r="D13" s="42">
+      <c r="D13" s="38">
         <v>31748</v>
       </c>
-      <c r="E13" s="41">
+      <c r="E13" s="37">
         <v>127.9</v>
       </c>
-      <c r="F13" s="41">
+      <c r="F13" s="37">
         <v>147.69999999999999</v>
       </c>
-      <c r="G13" s="41">
+      <c r="G13" s="37">
         <v>183.4</v>
       </c>
-      <c r="H13" s="41">
+      <c r="H13" s="37">
         <v>117.4</v>
       </c>
-      <c r="I13" s="41">
+      <c r="I13" s="37">
         <v>141.80000000000001</v>
       </c>
-      <c r="J13" s="41">
+      <c r="J13" s="37">
         <v>175.6</v>
       </c>
-      <c r="K13" s="41">
+      <c r="K13" s="37">
         <v>210.7</v>
       </c>
-      <c r="L13" s="41">
+      <c r="L13" s="37">
         <v>234.7</v>
       </c>
-      <c r="M13" s="41">
+      <c r="M13" s="37">
         <v>292.60000000000002</v>
       </c>
     </row>
@@ -21510,40 +21510,40 @@
       <c r="A14" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="41">
+      <c r="B14" s="37">
         <v>105938</v>
       </c>
-      <c r="C14" s="41">
+      <c r="C14" s="37">
         <v>103451</v>
       </c>
-      <c r="D14" s="42">
+      <c r="D14" s="38">
         <v>110801</v>
       </c>
-      <c r="E14" s="41">
+      <c r="E14" s="37">
         <v>185.3</v>
       </c>
-      <c r="F14" s="41">
+      <c r="F14" s="37">
         <v>213.3</v>
       </c>
-      <c r="G14" s="41">
+      <c r="G14" s="37">
         <v>234.1</v>
       </c>
-      <c r="H14" s="41">
+      <c r="H14" s="37">
         <v>176.8</v>
       </c>
-      <c r="I14" s="41">
+      <c r="I14" s="37">
         <v>206.2</v>
       </c>
-      <c r="J14" s="41">
+      <c r="J14" s="37">
         <v>224</v>
       </c>
-      <c r="K14" s="41">
+      <c r="K14" s="37">
         <v>274.3</v>
       </c>
-      <c r="L14" s="41">
+      <c r="L14" s="37">
         <v>321.2</v>
       </c>
-      <c r="M14" s="41">
+      <c r="M14" s="37">
         <v>357.1</v>
       </c>
     </row>
@@ -21551,40 +21551,40 @@
       <c r="A15" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="41">
+      <c r="B15" s="37">
         <v>5691</v>
       </c>
-      <c r="C15" s="41">
+      <c r="C15" s="37">
         <v>6066</v>
       </c>
-      <c r="D15" s="42">
+      <c r="D15" s="38">
         <v>6927</v>
       </c>
-      <c r="E15" s="41">
+      <c r="E15" s="37">
         <v>30.5</v>
       </c>
-      <c r="F15" s="41">
+      <c r="F15" s="37">
         <v>32</v>
       </c>
-      <c r="G15" s="41">
+      <c r="G15" s="37">
         <v>38.5</v>
       </c>
-      <c r="H15" s="41">
+      <c r="H15" s="37">
         <v>27.1</v>
       </c>
-      <c r="I15" s="41">
+      <c r="I15" s="37">
         <v>31.1</v>
       </c>
-      <c r="J15" s="41">
+      <c r="J15" s="37">
         <v>34.5</v>
       </c>
-      <c r="K15" s="41">
+      <c r="K15" s="37">
         <v>28.5</v>
       </c>
-      <c r="L15" s="41">
+      <c r="L15" s="37">
         <v>31.3</v>
       </c>
-      <c r="M15" s="41">
+      <c r="M15" s="37">
         <v>43.2</v>
       </c>
     </row>
@@ -21592,40 +21592,40 @@
       <c r="A16" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="41">
+      <c r="B16" s="37">
         <v>38381</v>
       </c>
-      <c r="C16" s="41">
+      <c r="C16" s="37">
         <v>34595</v>
       </c>
-      <c r="D16" s="42">
+      <c r="D16" s="38">
         <v>37478</v>
       </c>
-      <c r="E16" s="41">
+      <c r="E16" s="37">
         <v>82.3</v>
       </c>
-      <c r="F16" s="41">
+      <c r="F16" s="37">
         <v>81.2</v>
       </c>
-      <c r="G16" s="41">
+      <c r="G16" s="37">
         <v>111.3</v>
       </c>
-      <c r="H16" s="41">
+      <c r="H16" s="37">
         <v>68.2</v>
       </c>
-      <c r="I16" s="41">
+      <c r="I16" s="37">
         <v>77</v>
       </c>
-      <c r="J16" s="41">
+      <c r="J16" s="37">
         <v>93.3</v>
       </c>
-      <c r="K16" s="41">
+      <c r="K16" s="37">
         <v>262.5</v>
       </c>
-      <c r="L16" s="41">
+      <c r="L16" s="37">
         <v>292.60000000000002</v>
       </c>
-      <c r="M16" s="41">
+      <c r="M16" s="37">
         <v>347.1</v>
       </c>
     </row>
@@ -21633,40 +21633,40 @@
       <c r="A17" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="41">
+      <c r="B17" s="37">
         <v>18761</v>
       </c>
-      <c r="C17" s="41">
+      <c r="C17" s="37">
         <v>17802</v>
       </c>
-      <c r="D17" s="42">
+      <c r="D17" s="38">
         <v>20443</v>
       </c>
-      <c r="E17" s="41">
+      <c r="E17" s="37">
         <v>12.3</v>
       </c>
-      <c r="F17" s="41">
+      <c r="F17" s="37">
         <v>13.9</v>
       </c>
-      <c r="G17" s="41">
+      <c r="G17" s="37">
         <v>19.600000000000001</v>
       </c>
-      <c r="H17" s="41">
+      <c r="H17" s="37">
         <v>10.6</v>
       </c>
-      <c r="I17" s="41">
+      <c r="I17" s="37">
         <v>12.9</v>
       </c>
-      <c r="J17" s="41">
+      <c r="J17" s="37">
         <v>17.100000000000001</v>
       </c>
-      <c r="K17" s="41">
+      <c r="K17" s="37">
         <v>26.9</v>
       </c>
-      <c r="L17" s="41">
+      <c r="L17" s="37">
         <v>31</v>
       </c>
-      <c r="M17" s="41">
+      <c r="M17" s="37">
         <v>42.6</v>
       </c>
     </row>
@@ -21683,12 +21683,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21870,15 +21867,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F73EA17-884A-4BD0-A35A-DA27C5309908}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B151E57-6ACC-4260-8927-636EE7EC59B8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -21902,10 +21903,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B151E57-6ACC-4260-8927-636EE7EC59B8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F73EA17-884A-4BD0-A35A-DA27C5309908}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>